<commit_message>
Allow empty lines in app import Excel definitions file
</commit_message>
<xml_diff>
--- a/testdata/tasks.xlsx
+++ b/testdata/tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/goran/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F0D8E0-8F89-2A4E-9CD1-B6481F2C05F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FFE00D-1D5C-C846-A743-E6F683EFD766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="35840" windowHeight="14420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-52000" yWindow="800" windowWidth="35840" windowHeight="14420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ctrl-Q task import 1" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="132">
   <si>
     <t>Task counter</t>
   </si>
@@ -387,9 +387,6 @@
   </si>
   <si>
     <t>newapp-3</t>
-  </si>
-  <si>
-    <t>C:/tools/ctrl-q/testdata/</t>
   </si>
   <si>
     <t>When task A successful</t>
@@ -2372,7 +2369,7 @@
         <v>80</v>
       </c>
       <c r="AL13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AM13" t="s">
         <v>87</v>
@@ -2491,7 +2488,7 @@
         <v>80</v>
       </c>
       <c r="AL14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AM14" t="s">
         <v>88</v>
@@ -2507,9 +2504,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2549,13 +2546,13 @@
         <v>105</v>
       </c>
       <c r="H1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I1" t="s">
         <v>125</v>
       </c>
-      <c r="I1" t="s">
-        <v>126</v>
-      </c>
       <c r="J1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -2581,18 +2578,18 @@
         <v>118</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2" t="s">
         <v>127</v>
       </c>
-      <c r="I2" t="s">
-        <v>128</v>
-      </c>
       <c r="J2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H3" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -2603,7 +2600,7 @@
         <v>107</v>
       </c>
       <c r="C4" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="D4" t="s">
         <v>111</v>
@@ -2619,10 +2616,10 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -2645,13 +2642,13 @@
         <v>113</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I5" t="s">
         <v>127</v>
       </c>
-      <c r="I5" t="s">
-        <v>128</v>
-      </c>
       <c r="J5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Doc update wrt 3.7.0
</commit_message>
<xml_diff>
--- a/testdata/tasks.xlsx
+++ b/testdata/tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/goran/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FFE00D-1D5C-C846-A743-E6F683EFD766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AF65EC-4385-3140-B4D3-EB95A834805E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-52000" yWindow="800" windowWidth="35840" windowHeight="14420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-52000" yWindow="800" windowWidth="39320" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ctrl-Q task import 1" sheetId="4" r:id="rId1"/>
@@ -804,11 +804,11 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -821,9 +821,7 @@
     <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18.5" customWidth="1"/>
     <col min="17" max="17" width="26.5" customWidth="1"/>
-    <col min="22" max="33" width="0" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="0" hidden="1" customWidth="1"/>
+    <col min="22" max="35" width="10.83203125" customWidth="1"/>
     <col min="38" max="38" width="21.6640625" customWidth="1"/>
     <col min="39" max="39" width="35.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2504,9 +2502,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
feat(app-import): Add more options for publishing apps Implements #234
</commit_message>
<xml_diff>
--- a/testdata/tasks.xlsx
+++ b/testdata/tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/goran/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AF65EC-4385-3140-B4D3-EB95A834805E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107EF525-30E8-C14E-8DA7-04D5309F11A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-52000" yWindow="800" windowWidth="39320" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2600" windowWidth="35840" windowHeight="19800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ctrl-Q task import 1" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="137">
   <si>
     <t>Task counter</t>
   </si>
@@ -417,6 +417,21 @@
   </si>
   <si>
     <t>9143a1bf-abc3-46f4-8dcb-a1a0ea35860a</t>
+  </si>
+  <si>
+    <t>Publish options</t>
+  </si>
+  <si>
+    <t>delete-publish</t>
+  </si>
+  <si>
+    <t>publish-replace</t>
+  </si>
+  <si>
+    <t>publish-another</t>
+  </si>
+  <si>
+    <t>Reload task of App 1</t>
   </si>
 </sst>
 </file>
@@ -802,18 +817,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1908950-014B-5543-A83E-C294E0CD8CA9}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:AM14"/>
+  <dimension ref="A1:AM16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="44.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="52.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" customWidth="1"/>
     <col min="5" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
@@ -953,10 +969,10 @@
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>41</v>
+        <v>136</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -1185,97 +1201,97 @@
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="b">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" t="s">
-        <v>49</v>
+      <c r="F4">
+        <v>1440</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>49</v>
-      </c>
-      <c r="I4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J4" t="s">
-        <v>49</v>
+        <v>119</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="L4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="M4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="N4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="P4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="Q4" t="s">
-        <v>49</v>
-      </c>
-      <c r="R4">
-        <v>2</v>
+        <v>48</v>
+      </c>
+      <c r="R4" t="s">
+        <v>49</v>
       </c>
       <c r="S4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T4" t="s">
-        <v>62</v>
-      </c>
-      <c r="U4" t="b">
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="U4" t="s">
+        <v>49</v>
       </c>
       <c r="V4" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="W4" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="X4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="Y4" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="Z4" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="AA4" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="AB4" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="AC4" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="AD4" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="AE4" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="AF4" t="s">
         <v>49</v>
@@ -1307,94 +1323,94 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5">
+        <v>49</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L5" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5" t="s">
+        <v>49</v>
+      </c>
+      <c r="P5" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>49</v>
+      </c>
+      <c r="R5">
         <v>1</v>
       </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1440</v>
-      </c>
-      <c r="G5">
+      <c r="S5" t="s">
+        <v>50</v>
+      </c>
+      <c r="T5" t="s">
+        <v>51</v>
+      </c>
+      <c r="U5" t="b">
         <v>0</v>
       </c>
-      <c r="H5" t="s">
-        <v>120</v>
-      </c>
-      <c r="I5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K5" t="s">
-        <v>69</v>
-      </c>
-      <c r="L5" t="s">
-        <v>70</v>
-      </c>
-      <c r="M5" t="s">
-        <v>71</v>
-      </c>
-      <c r="N5" t="s">
-        <v>72</v>
-      </c>
-      <c r="O5" t="s">
-        <v>46</v>
-      </c>
-      <c r="P5" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>74</v>
-      </c>
-      <c r="R5" t="s">
-        <v>49</v>
-      </c>
-      <c r="S5" t="s">
-        <v>49</v>
-      </c>
-      <c r="T5" t="s">
-        <v>49</v>
-      </c>
-      <c r="U5" t="s">
-        <v>49</v>
-      </c>
       <c r="V5" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="W5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="X5" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="Y5" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="Z5" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="AA5" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="AB5" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="AC5" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="AD5" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="AE5" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="AF5" t="s">
         <v>49</v>
@@ -1423,97 +1439,97 @@
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" t="s">
+        <v>49</v>
+      </c>
+      <c r="N6" t="s">
+        <v>49</v>
+      </c>
+      <c r="O6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P6" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>49</v>
+      </c>
+      <c r="R6">
         <v>2</v>
       </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1440</v>
-      </c>
-      <c r="G6">
+      <c r="S6" t="s">
+        <v>50</v>
+      </c>
+      <c r="T6" t="s">
+        <v>62</v>
+      </c>
+      <c r="U6" t="b">
         <v>0</v>
       </c>
-      <c r="H6" t="s">
-        <v>121</v>
-      </c>
-      <c r="I6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" t="s">
-        <v>76</v>
-      </c>
-      <c r="M6" t="s">
-        <v>77</v>
-      </c>
-      <c r="N6" t="s">
-        <v>45</v>
-      </c>
-      <c r="O6" t="s">
-        <v>46</v>
-      </c>
-      <c r="P6" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>49</v>
-      </c>
-      <c r="R6" t="s">
-        <v>49</v>
-      </c>
-      <c r="S6" t="s">
-        <v>49</v>
-      </c>
-      <c r="T6" t="s">
-        <v>49</v>
-      </c>
-      <c r="U6" t="s">
-        <v>49</v>
-      </c>
       <c r="V6" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="W6" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="X6" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="Y6" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="Z6" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="AA6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="AB6" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="AC6" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="AD6" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="AE6" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="AF6" t="s">
         <v>49</v>
@@ -1542,16 +1558,16 @@
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" t="s">
-        <v>90</v>
+        <v>68</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -1560,7 +1576,7 @@
         <v>1440</v>
       </c>
       <c r="G7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H7" t="s">
         <v>120</v>
@@ -1569,28 +1585,28 @@
         <v>0</v>
       </c>
       <c r="J7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" t="s">
         <v>69</v>
       </c>
       <c r="L7" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="M7" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="N7" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="O7" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="P7" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="Q7" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="R7" t="s">
         <v>49</v>
@@ -1664,46 +1680,46 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" t="s">
-        <v>49</v>
+        <v>75</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1440</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J8" t="s">
-        <v>49</v>
+        <v>121</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="L8" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="M8" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="N8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="O8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="P8" t="s">
         <v>49</v>
@@ -1711,47 +1727,47 @@
       <c r="Q8" t="s">
         <v>49</v>
       </c>
-      <c r="R8">
-        <v>1</v>
+      <c r="R8" t="s">
+        <v>49</v>
       </c>
       <c r="S8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T8" t="s">
-        <v>83</v>
-      </c>
-      <c r="U8" t="b">
-        <v>1</v>
+        <v>49</v>
+      </c>
+      <c r="U8" t="s">
+        <v>49</v>
       </c>
       <c r="V8" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="W8" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="X8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="Y8" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="Z8" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="AA8" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="AB8" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="AC8" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="AD8" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="AE8" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="AF8" t="s">
         <v>49</v>
@@ -1780,97 +1796,97 @@
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" t="s">
-        <v>49</v>
+        <v>90</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1440</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>49</v>
-      </c>
-      <c r="I9" t="s">
-        <v>49</v>
-      </c>
-      <c r="J9" t="s">
-        <v>49</v>
+        <v>120</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="L9" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="M9" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="N9" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="O9" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="P9" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="Q9" t="s">
-        <v>49</v>
-      </c>
-      <c r="R9">
-        <v>2</v>
+        <v>85</v>
+      </c>
+      <c r="R9" t="s">
+        <v>49</v>
       </c>
       <c r="S9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="T9" t="s">
-        <v>96</v>
-      </c>
-      <c r="U9" t="b">
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="U9" t="s">
+        <v>49</v>
       </c>
       <c r="V9" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="W9" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="X9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="Y9" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="Z9" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="AA9" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="AB9" t="s">
-        <v>99</v>
+        <v>49</v>
       </c>
       <c r="AC9" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="AD9" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="AE9" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="AF9" t="s">
         <v>49</v>
@@ -1899,7 +1915,7 @@
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>49</v>
@@ -1950,16 +1966,16 @@
         <v>49</v>
       </c>
       <c r="R10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S10" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="T10" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="U10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10" t="s">
         <v>94</v>
@@ -1971,37 +1987,37 @@
         <v>54</v>
       </c>
       <c r="Y10" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="Z10" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="AA10" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="AB10" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="AC10" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="AD10" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="AE10" t="s">
-        <v>49</v>
-      </c>
-      <c r="AF10">
-        <v>0</v>
-      </c>
-      <c r="AG10">
-        <v>360</v>
-      </c>
-      <c r="AH10">
-        <v>0</v>
-      </c>
-      <c r="AI10">
-        <v>0</v>
+        <v>61</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>49</v>
       </c>
       <c r="AJ10" t="s">
         <v>49</v>
@@ -2018,7 +2034,7 @@
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
         <v>49</v>
@@ -2069,46 +2085,46 @@
         <v>49</v>
       </c>
       <c r="R11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="T11" t="s">
-        <v>49</v>
-      </c>
-      <c r="U11" t="s">
-        <v>49</v>
+        <v>96</v>
+      </c>
+      <c r="U11" t="b">
+        <v>0</v>
       </c>
       <c r="V11" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="W11" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="X11" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="Y11" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="Z11" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="AA11" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="AB11" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="AC11" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="AD11" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="AE11" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="AF11" t="s">
         <v>49</v>
@@ -2122,22 +2138,22 @@
       <c r="AI11" t="s">
         <v>49</v>
       </c>
-      <c r="AJ11">
-        <v>1</v>
+      <c r="AJ11" t="s">
+        <v>49</v>
       </c>
       <c r="AK11" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="AL11" t="s">
-        <v>40</v>
-      </c>
-      <c r="AM11">
-        <v>2</v>
+        <v>49</v>
+      </c>
+      <c r="AM11" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
         <v>49</v>
@@ -2191,22 +2207,22 @@
         <v>3</v>
       </c>
       <c r="S12" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="T12" t="s">
-        <v>49</v>
-      </c>
-      <c r="U12" t="s">
-        <v>49</v>
+        <v>100</v>
+      </c>
+      <c r="U12" t="b">
+        <v>0</v>
       </c>
       <c r="V12" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="W12" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="X12" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="Y12" t="s">
         <v>49</v>
@@ -2229,34 +2245,34 @@
       <c r="AE12" t="s">
         <v>49</v>
       </c>
-      <c r="AF12" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG12" t="s">
-        <v>49</v>
-      </c>
-      <c r="AH12" t="s">
-        <v>49</v>
-      </c>
-      <c r="AI12" t="s">
-        <v>49</v>
-      </c>
-      <c r="AJ12">
-        <v>2</v>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12">
+        <v>360</v>
+      </c>
+      <c r="AH12">
+        <v>0</v>
+      </c>
+      <c r="AI12">
+        <v>0</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>49</v>
       </c>
       <c r="AK12" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="AL12" t="s">
-        <v>81</v>
-      </c>
-      <c r="AM12">
-        <v>1</v>
+        <v>49</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
         <v>49</v>
@@ -2361,21 +2377,21 @@
         <v>49</v>
       </c>
       <c r="AJ13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AK13" t="s">
         <v>80</v>
       </c>
       <c r="AL13" t="s">
-        <v>122</v>
-      </c>
-      <c r="AM13" t="s">
-        <v>87</v>
+        <v>40</v>
+      </c>
+      <c r="AM13">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
         <v>49</v>
@@ -2480,15 +2496,253 @@
         <v>49</v>
       </c>
       <c r="AJ14">
+        <v>2</v>
+      </c>
+      <c r="AK14" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL14" t="s">
+        <v>81</v>
+      </c>
+      <c r="AM14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" t="s">
+        <v>49</v>
+      </c>
+      <c r="J15" t="s">
+        <v>49</v>
+      </c>
+      <c r="K15" t="s">
+        <v>49</v>
+      </c>
+      <c r="L15" t="s">
+        <v>49</v>
+      </c>
+      <c r="M15" t="s">
+        <v>49</v>
+      </c>
+      <c r="N15" t="s">
+        <v>49</v>
+      </c>
+      <c r="O15" t="s">
+        <v>49</v>
+      </c>
+      <c r="P15" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>49</v>
+      </c>
+      <c r="R15">
+        <v>3</v>
+      </c>
+      <c r="S15" t="s">
+        <v>49</v>
+      </c>
+      <c r="T15" t="s">
+        <v>49</v>
+      </c>
+      <c r="U15" t="s">
+        <v>49</v>
+      </c>
+      <c r="V15" t="s">
+        <v>49</v>
+      </c>
+      <c r="W15" t="s">
+        <v>49</v>
+      </c>
+      <c r="X15" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ15">
+        <v>3</v>
+      </c>
+      <c r="AK15" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" t="s">
+        <v>49</v>
+      </c>
+      <c r="K16" t="s">
+        <v>49</v>
+      </c>
+      <c r="L16" t="s">
+        <v>49</v>
+      </c>
+      <c r="M16" t="s">
+        <v>49</v>
+      </c>
+      <c r="N16" t="s">
+        <v>49</v>
+      </c>
+      <c r="O16" t="s">
+        <v>49</v>
+      </c>
+      <c r="P16" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>49</v>
+      </c>
+      <c r="R16">
+        <v>3</v>
+      </c>
+      <c r="S16" t="s">
+        <v>49</v>
+      </c>
+      <c r="T16" t="s">
+        <v>49</v>
+      </c>
+      <c r="U16" t="s">
+        <v>49</v>
+      </c>
+      <c r="V16" t="s">
+        <v>49</v>
+      </c>
+      <c r="W16" t="s">
+        <v>49</v>
+      </c>
+      <c r="X16" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AJ16">
         <v>4</v>
       </c>
-      <c r="AK14" t="s">
+      <c r="AK16" t="s">
         <v>80</v>
       </c>
-      <c r="AL14" t="s">
+      <c r="AL16" t="s">
         <v>123</v>
       </c>
-      <c r="AM14" t="s">
+      <c r="AM16" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2500,11 +2754,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCB302AA-7244-6143-A82A-1F338369BBC6}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2519,9 +2773,10 @@
     <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -2552,28 +2807,31 @@
       <c r="J1" t="s">
         <v>128</v>
       </c>
+      <c r="K1" t="s">
+        <v>132</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
         <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="s">
         <v>113</v>
       </c>
       <c r="G2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>126</v>
@@ -2582,70 +2840,225 @@
         <v>127</v>
       </c>
       <c r="J2" t="s">
-        <v>129</v>
+        <v>131</v>
+      </c>
+      <c r="K2" t="s">
+        <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H3" s="1" t="s">
-        <v>126</v>
-      </c>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
         <v>109</v>
       </c>
       <c r="D4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G4" t="s">
         <v>117</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="I4" t="s">
         <v>127</v>
       </c>
       <c r="J4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>113</v>
+      </c>
+      <c r="G6" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J6" t="s">
+        <v>129</v>
+      </c>
+      <c r="K6" t="s">
+        <v>134</v>
+      </c>
+      <c r="L6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I7" t="s">
+        <v>127</v>
+      </c>
+      <c r="J7" t="s">
+        <v>129</v>
+      </c>
+      <c r="K7" t="s">
+        <v>135</v>
+      </c>
+      <c r="L7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I8" t="s">
+        <v>127</v>
+      </c>
+      <c r="J8" t="s">
+        <v>131</v>
+      </c>
+      <c r="K8" t="s">
+        <v>134</v>
+      </c>
+      <c r="L8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H9" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>114</v>
+      </c>
+      <c r="G10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" t="s">
+        <v>127</v>
+      </c>
+      <c r="J10" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
         <v>108</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C11" t="s">
         <v>109</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D11" t="s">
         <v>112</v>
       </c>
-      <c r="E5" t="b">
+      <c r="E11" t="b">
         <v>0</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F11" t="s">
         <v>113</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I11" t="s">
         <v>127</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J11" t="s">
         <v>131</v>
       </c>
     </row>

</xml_diff>